<commit_message>
add cause_category to Lebensmittel.py
</commit_message>
<xml_diff>
--- a/Patterns_fuer_Warnungskategorien.xlsx
+++ b/Patterns_fuer_Warnungskategorien.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katja\Documents\Studium Angewandte Bioinformatik\5. Semester\BIGD\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katja\Documents\GitHub\BIGD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1379BDBF-D78F-4769-850B-52A4346FD8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D323A3F-FB54-4EB1-91A0-B688151EDF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{577AA07A-8509-4834-9D68-7A79915BCD33}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{577AA07A-8509-4834-9D68-7A79915BCD33}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -550,37 +550,37 @@
     <t>(in python: import re)</t>
   </si>
   <si>
-    <t>(.Listeri.*) | (Salmonell.*) | (Patulin.*) | (.*(T|t)oxin.*)</t>
-  </si>
-  <si>
-    <t>| (Pseudomon.*) | (Schimmel.*) | (Escherichia.*)</t>
-  </si>
-  <si>
-    <t>| ((M|m)ikro.*) | (Ba(c|z)ill.*) | (Hefe.*)</t>
-  </si>
-  <si>
     <t>Fremdkörper/-stoffe</t>
   </si>
   <si>
-    <t xml:space="preserve">(.*(F|f)remd.*) | (Glas.*) | (Metall.*) </t>
-  </si>
-  <si>
-    <t>| (Kunststoff.*) | (Stein.*)</t>
-  </si>
-  <si>
-    <t>(.*(A|a)llerg.*) | (.*nuss) | (Senf.*) | (Milch.*)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(.*(W|w)ert.*) | (.*(G|g)ehalt.*) | ((R|r)ückst.*) | (.*(M|m)enge.*) </t>
-  </si>
-  <si>
     <t>zu hohe Konzentration, gesundheitsschädliche Wirkung</t>
   </si>
   <si>
-    <t>| (Arznei.*) | (Nachweis.*) | ((G|g)esund.*) | ((G|g)esetz.*) | (krebs.*)</t>
-  </si>
-  <si>
-    <t>| (Befund.*) | ((G|g)ef(a|ä)hr.*) | (zugelassen.*)</t>
+    <t>(Listeri.*)|(Salmonell.*)|(Patulin.*)|(.*(T|t)oxin.*)</t>
+  </si>
+  <si>
+    <t>|(Pseudomon.*)|(Schimmel.*)|(Escherichia.*)</t>
+  </si>
+  <si>
+    <t>|((M|m)ikro.*)|(Ba(c|z)ill.*)|(Hefe.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(.*(F|f)remd.*)|(Glas.*)|(Metall.*) </t>
+  </si>
+  <si>
+    <t>|(Kunststoff.*)|(Stein.*)</t>
+  </si>
+  <si>
+    <t>(.*(A|a)llerg.*)|(.*nuss)|(Senf.*)|(Milch.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(.*(W|w)ert.*)|(.*(G|g)ehalt.*)|((R|r)ückst.*)|(.*(M|m)enge.*) </t>
+  </si>
+  <si>
+    <t>|(Arznei.*)|(Nachweis.*)|((G|g)esund.*)|((G|g)esetz.*)|(krebs.*)</t>
+  </si>
+  <si>
+    <t>|(Befund.*)|((G|g)ef(a|ä)hr.*)|(zugelassen.*)</t>
   </si>
 </sst>
 </file>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D4D05B-D75B-4F8F-841C-8EFA876F30AA}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -976,7 +976,7 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -993,16 +993,16 @@
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1010,10 +1010,10 @@
         <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
         <v>183</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
         <v>184</v>
@@ -1211,7 +1211,7 @@
         <v>53</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
kleine Verbesserung der Patterns
</commit_message>
<xml_diff>
--- a/Patterns_fuer_Warnungskategorien.xlsx
+++ b/Patterns_fuer_Warnungskategorien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katja\Documents\GitHub\BIGD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D323A3F-FB54-4EB1-91A0-B688151EDF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C8847C-58EA-4137-B67E-DA22AD634D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{577AA07A-8509-4834-9D68-7A79915BCD33}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="14400" windowHeight="7270" xr2:uid="{577AA07A-8509-4834-9D68-7A79915BCD33}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -571,9 +571,6 @@
     <t>|(Kunststoff.*)|(Stein.*)</t>
   </si>
   <si>
-    <t>(.*(A|a)llerg.*)|(.*nuss)|(Senf.*)|(Milch.*)</t>
-  </si>
-  <si>
     <t xml:space="preserve">(.*(W|w)ert.*)|(.*(G|g)ehalt.*)|((R|r)ückst.*)|(.*(M|m)enge.*) </t>
   </si>
   <si>
@@ -581,6 +578,9 @@
   </si>
   <si>
     <t>|(Befund.*)|((G|g)ef(a|ä)hr.*)|(zugelassen.*)</t>
+  </si>
+  <si>
+    <t>(.*(A|a)llerg.*)|(.*nuss)|(Senf.*)|(Milch.*)|(Sesam.*)</t>
   </si>
 </sst>
 </file>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D4D05B-D75B-4F8F-841C-8EFA876F30AA}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -999,10 +999,10 @@
         <v>179</v>
       </c>
       <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" t="s">
         <v>181</v>
-      </c>
-      <c r="E2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1016,7 +1016,7 @@
         <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1024,7 +1024,7 @@
         <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">

</xml_diff>